<commit_message>
update master meeting presentation
</commit_message>
<xml_diff>
--- a/Simulator/weight_calc.xlsx
+++ b/Simulator/weight_calc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Personal\master\Master_git\Master\Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -379,12 +379,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,6 +421,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,8 +433,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,7 +496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -571,7 +570,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2227,46 +2225,28 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.2363370914723325E-2"/>
+          <c:y val="3.9007081307008071E-2"/>
+          <c:w val="0.87396045504273812"/>
+          <c:h val="0.8232331425606908"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>UR</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2347,9 +2327,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.42499999999999999</c:v>
                 </c:pt>
@@ -2374,9 +2351,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>8.4</c:v>
                 </c:pt>
@@ -2483,9 +2457,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.14399999999999999</c:v>
                 </c:pt>
@@ -2510,9 +2481,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>4.75</c:v>
                 </c:pt>
@@ -2570,6 +2538,73 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Accumulated Length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> (meters)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36020590137521713"/>
+              <c:y val="0.91613477518993269"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
@@ -2632,6 +2667,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Accumuluted Weight (Kg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2681,6 +2772,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.71673170242044826"/>
+          <c:y val="0.55053092351289346"/>
+          <c:w val="0.23889108427795061"/>
+          <c:h val="0.281916490222681"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5070,8 +5202,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
@@ -5079,7 +5211,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>400049</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5367,7 +5499,7 @@
   <dimension ref="B3:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J21" activeCellId="1" sqref="K21 J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,57 +5558,51 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>3.7</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <f>D5*E5</f>
         <v>0.32929999999999998</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <f>D5/E5</f>
         <v>41.573033707865171</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <f>E5/D5*100</f>
         <v>2.4054054054054053</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="19">
+      <c r="B6" s="21"/>
+      <c r="C6" s="17">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>8.4</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0.42499999999999999</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <f t="shared" ref="F6:F16" si="1">D6*E6</f>
         <v>3.57</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <f t="shared" ref="G6:G16" si="2">D6/E6</f>
         <v>19.764705882352942</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <f t="shared" ref="H6:H16" si="3">E6/D6*100</f>
         <v>5.0595238095238093</v>
       </c>
@@ -5490,25 +5616,25 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="19">
+      <c r="B7" s="21"/>
+      <c r="C7" s="17">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>2.2749999999999999</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>0.39200000000000002</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <f t="shared" si="1"/>
         <v>0.89180000000000004</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <f t="shared" si="2"/>
         <v>5.8035714285714279</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <f t="shared" si="3"/>
         <v>17.230769230769234</v>
       </c>
@@ -5522,25 +5648,25 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="19">
+      <c r="B8" s="21"/>
+      <c r="C8" s="17">
         <v>4</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>1.2190000000000001</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>0.11336700000000001</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <f t="shared" si="2"/>
         <v>13.107526881720432</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <f t="shared" si="3"/>
         <v>7.6292042657916319</v>
       </c>
@@ -5554,25 +5680,25 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="19">
+      <c r="B9" s="21"/>
+      <c r="C9" s="17">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>1.2190000000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>0.11580500000000001</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <f t="shared" si="2"/>
         <v>12.831578947368422</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <f t="shared" si="3"/>
         <v>7.7932731747333879</v>
       </c>
@@ -5586,25 +5712,25 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-      <c r="C10" s="20">
+      <c r="B10" s="22"/>
+      <c r="C10" s="18">
         <v>6</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>0.18790000000000001</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
         <v>1.5407800000000001E-2</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="11">
         <f t="shared" si="2"/>
         <v>2.2914634146341464</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <f t="shared" si="3"/>
         <v>43.640234167110165</v>
       </c>
@@ -5618,57 +5744,51 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <v>1</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>10.54</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>0.25700000000000001</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>2.70878</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="8">
         <f t="shared" si="2"/>
         <v>41.011673151750969</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <f t="shared" si="3"/>
         <v>2.4383301707779892</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="16">
+      <c r="B12" s="23"/>
+      <c r="C12" s="14">
         <v>2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
         <v>4.75</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>0.14399999999999999</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <f t="shared" si="1"/>
         <v>0.68399999999999994</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <f t="shared" si="2"/>
         <v>32.986111111111114</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <f t="shared" si="3"/>
         <v>3.0315789473684207</v>
       </c>
@@ -5682,25 +5802,25 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="16">
+      <c r="B13" s="23"/>
+      <c r="C13" s="14">
         <v>3</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
         <v>6.14</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>0.58499999999999996</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <f t="shared" si="1"/>
         <v>3.5918999999999994</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <f t="shared" si="2"/>
         <v>10.495726495726496</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <f t="shared" si="3"/>
         <v>9.5276872964169375</v>
       </c>
@@ -5714,25 +5834,25 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="16">
+      <c r="B14" s="23"/>
+      <c r="C14" s="14">
         <v>4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <v>0.16</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <f t="shared" si="1"/>
         <v>0.39200000000000002</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <f t="shared" si="2"/>
         <v>15.3125</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <f t="shared" si="3"/>
         <v>6.5306122448979584</v>
       </c>
@@ -5746,25 +5866,25 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="16">
+      <c r="B15" s="23"/>
+      <c r="C15" s="14">
         <v>5</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <v>2.06</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <v>0.32500000000000001</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
         <v>0.6695000000000001</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <f t="shared" si="2"/>
         <v>6.3384615384615381</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <f t="shared" si="3"/>
         <v>15.776699029126215</v>
       </c>
@@ -5778,25 +5898,25 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="17">
+      <c r="B16" s="24"/>
+      <c r="C16" s="15">
         <v>6</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <v>0.48799999999999999</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <f t="shared" si="1"/>
         <v>3.1719999999999998E-2</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="11">
         <f t="shared" si="2"/>
         <v>7.5076923076923077</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="12">
         <f t="shared" si="3"/>
         <v>13.319672131147541</v>
       </c>
@@ -5832,19 +5952,19 @@
       </c>
     </row>
     <row r="18" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="F18" s="24">
+      <c r="F18" s="19">
         <f>2.275*0.4/0.392</f>
         <v>2.3214285714285716</v>
       </c>
     </row>
     <row r="21" spans="4:19" x14ac:dyDescent="0.25">
       <c r="J21">
-        <f>(11.737+11.681)/2</f>
-        <v>11.709</v>
+        <f>(9.8785+7.7026)/2</f>
+        <v>8.7905499999999996</v>
       </c>
       <c r="K21">
-        <f>(1.7607+1.2619)/2</f>
-        <v>1.5112999999999999</v>
+        <f>(3.647+4.9386)/2</f>
+        <v>4.2927999999999997</v>
       </c>
       <c r="M21" t="s">
         <v>2</v>
@@ -5867,22 +5987,22 @@
       </c>
       <c r="M23">
         <f>I6*$J$21+$K$21-N22</f>
-        <v>6.4876249999999995</v>
+        <v>8.0287837499999988</v>
       </c>
       <c r="N23">
         <f>M23+N22</f>
-        <v>6.4876249999999995</v>
+        <v>8.0287837499999988</v>
       </c>
       <c r="Q23" t="s">
         <v>10</v>
       </c>
       <c r="R23">
         <f>I12*$J$21+$K$21-S22</f>
-        <v>3.1973959999999995</v>
+        <v>5.5586392</v>
       </c>
       <c r="S23">
         <f>R23+S22</f>
-        <v>3.1973959999999995</v>
+        <v>5.5586392</v>
       </c>
     </row>
     <row r="24" spans="4:19" x14ac:dyDescent="0.25">
@@ -5898,33 +6018,33 @@
       </c>
       <c r="I24">
         <f>G24*$J$21+$K$21-J23</f>
-        <v>6.1949000000000005</v>
+        <v>7.8090200000000003</v>
       </c>
       <c r="J24">
         <f>I24+J23</f>
-        <v>6.1949000000000005</v>
+        <v>7.8090200000000003</v>
       </c>
       <c r="L24" t="s">
         <v>11</v>
       </c>
       <c r="M24">
         <f>I7*$J$21+$K$21-N23</f>
-        <v>4.5899280000000005</v>
+        <v>3.4458956000000001</v>
       </c>
       <c r="N24">
         <f t="shared" ref="N24:N27" si="5">M24+N23</f>
-        <v>11.077553</v>
+        <v>11.474679349999999</v>
       </c>
       <c r="Q24" t="s">
         <v>11</v>
       </c>
       <c r="R24">
         <f t="shared" ref="R24:R27" si="6">I13*$J$21+$K$21-S23</f>
-        <v>6.8497649999999997</v>
+        <v>5.1424717500000003</v>
       </c>
       <c r="S24">
         <f t="shared" ref="S24:S27" si="7">R24+S23</f>
-        <v>10.047160999999999</v>
+        <v>10.70111095</v>
       </c>
     </row>
     <row r="25" spans="4:19" x14ac:dyDescent="0.25">
@@ -5940,33 +6060,33 @@
       </c>
       <c r="I25">
         <f t="shared" ref="I25:I27" si="8">G25*$J$21+$K$21-J24</f>
-        <v>8.1963000000000008</v>
+        <v>6.1533850000000001</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J28" si="9">I25+J24</f>
-        <v>14.391200000000001</v>
+        <f t="shared" ref="J25:J27" si="9">I25+J24</f>
+        <v>13.962405</v>
       </c>
       <c r="L25" t="s">
         <v>14</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M24:M27" si="10">I8*$J$21+$K$21-N24</f>
-        <v>1.0889369999999996</v>
+        <f t="shared" ref="M25:M27" si="10">I8*$J$21+$K$21-N24</f>
+        <v>0.81752115000000103</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
-        <v>12.16649</v>
+        <v>12.2922005</v>
       </c>
       <c r="Q25" t="s">
         <v>14</v>
       </c>
       <c r="R25">
         <f t="shared" si="6"/>
-        <v>1.8734400000000004</v>
+        <v>1.4064879999999995</v>
       </c>
       <c r="S25">
         <f t="shared" si="7"/>
-        <v>11.920601</v>
+        <v>12.10759895</v>
       </c>
     </row>
     <row r="26" spans="4:19" x14ac:dyDescent="0.25">
@@ -5974,7 +6094,7 @@
         <v>0.7</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26:G28" si="11">F26+G25</f>
+        <f t="shared" ref="G26:G27" si="11">F26+G25</f>
         <v>1.8</v>
       </c>
       <c r="H26" t="s">
@@ -5982,33 +6102,33 @@
       </c>
       <c r="I26">
         <f t="shared" si="8"/>
-        <v>8.1962999999999973</v>
+        <v>6.1533849999999966</v>
       </c>
       <c r="J26">
         <f t="shared" si="9"/>
-        <v>22.587499999999999</v>
+        <v>20.115789999999997</v>
       </c>
       <c r="L26" t="s">
         <v>13</v>
       </c>
       <c r="M26">
         <f t="shared" si="10"/>
-        <v>1.1123549999999991</v>
+        <v>0.83510224999999849</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
-        <v>13.278844999999999</v>
+        <v>13.127302749999998</v>
       </c>
       <c r="Q26" t="s">
         <v>13</v>
       </c>
       <c r="R26">
         <f t="shared" si="6"/>
-        <v>3.8054249999999996</v>
+        <v>2.8569287499999998</v>
       </c>
       <c r="S26">
         <f t="shared" si="7"/>
-        <v>15.726025999999999</v>
+        <v>14.9645277</v>
       </c>
     </row>
     <row r="27" spans="4:19" x14ac:dyDescent="0.25">
@@ -6024,33 +6144,33 @@
       </c>
       <c r="I27">
         <f t="shared" si="8"/>
-        <v>4.683600000000002</v>
+        <v>3.5162200000000041</v>
       </c>
       <c r="J27">
         <f t="shared" si="9"/>
-        <v>27.271100000000001</v>
+        <v>23.632010000000001</v>
       </c>
       <c r="L27" t="s">
         <v>12</v>
       </c>
       <c r="M27">
         <f t="shared" si="10"/>
-        <v>0.9601380000000006</v>
+        <v>0.72082510000000077</v>
       </c>
       <c r="N27">
         <f t="shared" si="5"/>
-        <v>14.238982999999999</v>
+        <v>13.848127849999999</v>
       </c>
       <c r="Q27" t="s">
         <v>12</v>
       </c>
       <c r="R27">
         <f t="shared" si="6"/>
-        <v>0.76108499999999957</v>
+        <v>0.57138574999999925</v>
       </c>
       <c r="S27">
         <f t="shared" si="7"/>
-        <v>16.487110999999999</v>
+        <v>15.535913449999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>